<commit_message>
Updated the test to handle screen rotation, screen resolution scenarios. Additional tap, long press methods added.
</commit_message>
<xml_diff>
--- a/AmazonShopping/Data/TestData.xlsx
+++ b/AmazonShopping/Data/TestData.xlsx
@@ -14,7 +14,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="11" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="22" uniqueCount="16">
   <si>
     <t>TestRun</t>
   </si>
@@ -34,9 +34,6 @@
     <t>user</t>
   </si>
   <si>
-    <t>search</t>
-  </si>
-  <si>
     <t>65-inch TV</t>
   </si>
   <si>
@@ -44,6 +41,27 @@
   </si>
   <si>
     <t>cbr@2222</t>
+  </si>
+  <si>
+    <t>rotateScreen</t>
+  </si>
+  <si>
+    <t>n</t>
+  </si>
+  <si>
+    <t>y</t>
+  </si>
+  <si>
+    <t>screenResolution</t>
+  </si>
+  <si>
+    <t>default</t>
+  </si>
+  <si>
+    <t>2,6</t>
+  </si>
+  <si>
+    <t>product</t>
   </si>
 </sst>
 </file>
@@ -489,7 +507,7 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
-  <dimension ref="A1:D4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="D2" sqref="D2"/>
@@ -500,15 +518,17 @@
     <col min="1" max="1" width="12.28515625" style="4" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="29.140625" style="4" bestFit="1" customWidth="1"/>
     <col min="3" max="3" width="16.42578125" style="4" bestFit="1" customWidth="1"/>
-    <col min="4" max="16384" width="13" style="4"/>
+    <col min="4" max="5" width="13" style="4"/>
+    <col min="6" max="6" width="16.5703125" style="4" bestFit="1" customWidth="1"/>
+    <col min="7" max="16384" width="13" style="4"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:4">
+    <row r="1" spans="1:6">
       <c r="A1" s="8" t="s">
         <v>0</v>
       </c>
     </row>
-    <row r="2" spans="1:4">
+    <row r="2" spans="1:6">
       <c r="A2" s="2" t="s">
         <v>1</v>
       </c>
@@ -519,10 +539,16 @@
         <v>4</v>
       </c>
       <c r="D2" s="6" t="s">
-        <v>6</v>
+        <v>15</v>
+      </c>
+      <c r="E2" s="6" t="s">
+        <v>9</v>
+      </c>
+      <c r="F2" s="6" t="s">
+        <v>12</v>
       </c>
     </row>
-    <row r="3" spans="1:4">
+    <row r="3" spans="1:6">
       <c r="A3" s="1">
         <v>1</v>
       </c>
@@ -533,21 +559,53 @@
         <v>3</v>
       </c>
       <c r="D3" s="3" t="s">
-        <v>7</v>
+        <v>6</v>
+      </c>
+      <c r="E3" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F3" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
-    <row r="4" spans="1:4">
+    <row r="4" spans="1:6">
       <c r="A4" s="1">
-        <v>0</v>
+        <v>1</v>
       </c>
       <c r="B4" s="7" t="s">
         <v>2</v>
       </c>
-      <c r="C4" s="7" t="s">
-        <v>9</v>
+      <c r="C4" s="5" t="s">
+        <v>3</v>
       </c>
       <c r="D4" s="3" t="s">
+        <v>6</v>
+      </c>
+      <c r="E4" s="3" t="s">
+        <v>11</v>
+      </c>
+      <c r="F4" s="3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6">
+      <c r="A5" s="1">
+        <v>0</v>
+      </c>
+      <c r="B5" s="7" t="s">
+        <v>2</v>
+      </c>
+      <c r="C5" s="7" t="s">
         <v>8</v>
+      </c>
+      <c r="D5" s="3" t="s">
+        <v>7</v>
+      </c>
+      <c r="E5" s="3" t="s">
+        <v>10</v>
+      </c>
+      <c r="F5" s="3" t="s">
+        <v>13</v>
       </c>
     </row>
   </sheetData>

</xml_diff>